<commit_message>
matplotlib waterfall chart unit test
</commit_message>
<xml_diff>
--- a/ProjectDataHandling/data_analysis/charts_waterfall_excel_layout_example.xlsx
+++ b/ProjectDataHandling/data_analysis/charts_waterfall_excel_layout_example.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\scripts_EDA\Project-Data-Handling\ProjectDataHandling\data_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Project_Management\Project-Data-Handling\ProjectDataHandling\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6217D7-6430-4EBF-8E89-EF9220B40DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14205"/>
+    <workbookView xWindow="-9690" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="50" iterateDelta="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -29,21 +41,12 @@
     <t>Label</t>
   </si>
   <si>
-    <t>measure</t>
-  </si>
-  <si>
-    <t>absolute</t>
-  </si>
-  <si>
     <t>initial</t>
   </si>
   <si>
     <t>after beg</t>
   </si>
   <si>
-    <t>relative</t>
-  </si>
-  <si>
     <t>cold test</t>
   </si>
   <si>
@@ -69,12 +72,21 @@
   </si>
   <si>
     <t>cold test 2</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
+    <t>rel</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,10 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,11 +406,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,112 +420,112 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>-2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-1</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>-10</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <f>+SUM(B2:B5)</f>
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>-3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>-8</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
+      <c r="A10" t="s">
+        <v>8</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>